<commit_message>
Commented out GeLuft lifetable code
</commit_message>
<xml_diff>
--- a/r_package/testing/comparison_lifetable_approaches/features_lifetable_approaches.xlsx
+++ b/r_package/testing/comparison_lifetable_approaches/features_lifetable_approaches.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12651"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,8 +18,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ACF: future development (long-term)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ACF: give user the option to replicate AirQ+ approach</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ACF: Probability of dying usually available for total mortality; number of natural and total deaths usually available</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>GeLuft</t>
   </si>
@@ -73,45 +154,65 @@
 of the next year</t>
   </si>
   <si>
-    <t>YLL's in the year of analysis are considered</t>
-  </si>
-  <si>
-    <t>Population projection</t>
-  </si>
-  <si>
-    <t>Population used and probability of death used 
-to calculate premature deaths align</t>
-  </si>
-  <si>
-    <t>___Population used</t>
-  </si>
-  <si>
     <t>Mid-year</t>
   </si>
   <si>
     <t>Entry</t>
   </si>
   <si>
-    <t>___Probability of death used</t>
-  </si>
-  <si>
-    <t>Mid-to-end-year</t>
-  </si>
-  <si>
-    <t>Start-to-end-year</t>
-  </si>
-  <si>
-    <t>Basis of population projection</t>
-  </si>
-  <si>
-    <t>Survival probability used</t>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Option: allow user to enter vector with non-natural deaths, or a correction factor (cf. ARE calculations in sheet "mort_all")</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Using the relationship modification_factor = 1 / rr_conc, the AirQ+ approach could allow more flexible ERF shapes</t>
+  </si>
+  <si>
+    <t>Probability used for population projection</t>
+  </si>
+  <si>
+    <t>Probability of surviving whole year</t>
+  </si>
+  <si>
+    <t>Population which is multiplied with survival probability</t>
+  </si>
+  <si>
+    <t>Calculated premature deaths are really deaths attributable to air pollution exposure</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No, something slightly different: the deaths from multiplying the mid-year population of 2019 with the probability of survival for a full year: e.g. the attributable deaths between July 2019 and July 2020 using the probability of surviving the year 2019</t>
+  </si>
+  <si>
+    <t>AirQ+ approach correct</t>
+  </si>
+  <si>
+    <t>Premature deaths due to air pollution in the year of analysis are assigned to year of analysis</t>
+  </si>
+  <si>
+    <t>YLL in year of analysis are correctly calculated</t>
+  </si>
+  <si>
+    <t>Yes, YLL = premature deaths / 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No, YLL = premature deaths </t>
+  </si>
+  <si>
+    <t>Option: default population input is mid-year population, put end/start of year population could be accepted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,13 +220,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,19 +260,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,200 +568,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="40.765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="48.21875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="40.77734375" style="2"/>
+    <col min="1" max="1" width="36.69140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.23046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.07421875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="33.07421875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="40.765625" style="1"/>
+    <col min="8" max="16384" width="40.765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="130.30000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>24</v>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" s="9" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>